<commit_message>
Historial y costos correctos
Se agrego el historial y se hizo coincidir con los costos del project plan
</commit_message>
<xml_diff>
--- a/PlanCostos_ProyectoFinal.xlsx
+++ b/PlanCostos_ProyectoFinal.xlsx
@@ -5,14 +5,15 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juan\Desktop\tareas\uag\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juan\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8085" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="History" sheetId="2" r:id="rId1"/>
+    <sheet name="Costos" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -23,108 +24,18 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>Juan</author>
-  </authors>
-  <commentList>
-    <comment ref="C22" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Juan:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-51 dias * 2
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C23" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Juan:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-44dias * 2 Horas</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C24" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Juan:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-51 dias * 2
-</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="42">
   <si>
     <t>Administración de proyectos</t>
   </si>
   <si>
-    <t>Tabla de valores</t>
-  </si>
-  <si>
     <t>Unidades</t>
   </si>
   <si>
     <t>Costos</t>
   </si>
   <si>
-    <t>Entrada</t>
-  </si>
-  <si>
     <t>Total</t>
   </si>
   <si>
@@ -140,9 +51,6 @@
     <t>Entrega</t>
   </si>
   <si>
-    <t>Costos de Implementación</t>
-  </si>
-  <si>
     <t>Presupuesto del cliente</t>
   </si>
   <si>
@@ -201,20 +109,63 @@
   </si>
   <si>
     <t>Tareas de PM</t>
+  </si>
+  <si>
+    <t>JAMR</t>
+  </si>
+  <si>
+    <t>IJE</t>
+  </si>
+  <si>
+    <t>JMC</t>
+  </si>
+  <si>
+    <t>GLG</t>
+  </si>
+  <si>
+    <t>Costo Mano de Obra</t>
+  </si>
+  <si>
+    <t>Costo Materiales</t>
+  </si>
+  <si>
+    <t>Fecha</t>
+  </si>
+  <si>
+    <t>Revision</t>
+  </si>
+  <si>
+    <t>Razón</t>
+  </si>
+  <si>
+    <t>Autor</t>
+  </si>
+  <si>
+    <t>Juan Mejia</t>
+  </si>
+  <si>
+    <t>Version inicial</t>
+  </si>
+  <si>
+    <t>Costo por ingeniero corregido</t>
+  </si>
+  <si>
+    <t>Agregado el Costo del servicio de la nuve</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="5">
+  <numFmts count="6">
     <numFmt numFmtId="164" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="167" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="168" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="170" formatCode="[$-409]d\-mmm\-yy;@"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -263,20 +214,15 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -319,8 +265,13 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="15">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -506,13 +457,44 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -559,10 +541,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="167" fontId="4" fillId="0" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -597,9 +575,6 @@
     <xf numFmtId="167" fontId="3" fillId="7" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="168" fontId="3" fillId="7" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="13" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -607,7 +582,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -618,8 +592,12 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="15" xfId="3"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
+    <cellStyle name="Celda de comprobación" xfId="3" builtinId="23"/>
     <cellStyle name="Millares" xfId="1" builtinId="3"/>
     <cellStyle name="Moneda" xfId="2" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -942,11 +920,95 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.125" customWidth="1"/>
+    <col min="2" max="2" width="30.25" customWidth="1"/>
+    <col min="3" max="3" width="34.5" customWidth="1"/>
+    <col min="4" max="4" width="41.125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="54" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="54" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="54" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="54" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="53">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="B2" s="55">
+        <v>43313</v>
+      </c>
+      <c r="C2" s="53" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="53" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="53">
+        <v>1.2</v>
+      </c>
+      <c r="B3" s="55">
+        <v>43314</v>
+      </c>
+      <c r="C3" s="53" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" s="53" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="53">
+        <v>1.4</v>
+      </c>
+      <c r="B4" s="55">
+        <v>43317</v>
+      </c>
+      <c r="C4" s="53" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" s="53" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="53"/>
+      <c r="B5" s="53"/>
+      <c r="C5" s="53"/>
+      <c r="D5" s="53"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G41"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -955,7 +1017,7 @@
     <col min="2" max="2" width="15.125" customWidth="1"/>
     <col min="3" max="3" width="13.875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="32.25" customWidth="1"/>
-    <col min="5" max="5" width="13.875" customWidth="1"/>
+    <col min="5" max="5" width="23.75" customWidth="1"/>
     <col min="6" max="6" width="17" customWidth="1"/>
     <col min="7" max="7" width="18.875" customWidth="1"/>
     <col min="11" max="11" width="11.125" bestFit="1" customWidth="1"/>
@@ -964,23 +1026,23 @@
     <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="4"/>
       <c r="B1" s="6"/>
-      <c r="C1" s="54" t="s">
-        <v>27</v>
-      </c>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
+      <c r="C1" s="50" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
     </row>
     <row r="2" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="4"/>
       <c r="B2" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" s="55" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="56"/>
-      <c r="E2" s="56"/>
+      <c r="C2" s="51" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
       <c r="F2" s="7">
         <v>3108514</v>
       </c>
@@ -988,11 +1050,11 @@
     <row r="3" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="4"/>
       <c r="B3" s="5"/>
-      <c r="C3" s="56" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="56"/>
-      <c r="E3" s="56"/>
+      <c r="C3" s="52" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="52"/>
+      <c r="E3" s="52"/>
       <c r="F3" s="7">
         <v>3116719</v>
       </c>
@@ -1000,11 +1062,11 @@
     <row r="4" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
-      <c r="C4" s="56" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" s="56"/>
-      <c r="E4" s="56"/>
+      <c r="C4" s="52" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="52"/>
+      <c r="E4" s="52"/>
       <c r="F4" s="7">
         <v>2600752</v>
       </c>
@@ -1012,11 +1074,11 @@
     <row r="5" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
-      <c r="C5" s="56" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" s="56"/>
-      <c r="E5" s="56"/>
+      <c r="C5" s="52" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="52"/>
+      <c r="E5" s="52"/>
       <c r="F5" s="7">
         <v>33108514</v>
       </c>
@@ -1024,12 +1086,12 @@
     <row r="6" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="4"/>
       <c r="B6" s="5"/>
-      <c r="C6" s="54" t="s">
+      <c r="C6" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="D6" s="54"/>
-      <c r="E6" s="54"/>
-      <c r="F6" s="54"/>
+      <c r="D6" s="50"/>
+      <c r="E6" s="50"/>
+      <c r="F6" s="50"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
@@ -1042,7 +1104,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>1</v>
+        <v>32</v>
       </c>
       <c r="B8" s="10"/>
       <c r="C8" s="11"/>
@@ -1053,10 +1115,10 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C9" s="14">
         <v>100</v>
@@ -1067,10 +1129,10 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C10" s="14">
         <v>100</v>
@@ -1081,10 +1143,10 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C11" s="14">
         <v>100</v>
@@ -1095,10 +1157,10 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C12" s="14">
         <v>150</v>
@@ -1108,28 +1170,24 @@
       <c r="G12" s="3"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="51" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" s="16">
-        <v>10000</v>
-      </c>
+      <c r="A13" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="10"/>
+      <c r="C13" s="11"/>
       <c r="D13" s="8"/>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="15" t="s">
-        <v>15</v>
+      <c r="A14" s="48" t="s">
+        <v>13</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C14" s="16">
-        <v>20000</v>
+        <v>10000</v>
       </c>
       <c r="D14" s="3"/>
       <c r="F14" s="3"/>
@@ -1137,13 +1195,13 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C15" s="16">
-        <v>2500</v>
+        <v>20000</v>
       </c>
       <c r="D15" s="3"/>
       <c r="F15" s="3"/>
@@ -1151,10 +1209,10 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C16" s="16">
         <v>5000</v>
@@ -1164,24 +1222,30 @@
       <c r="G16" s="3"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="53" t="s">
-        <v>5</v>
+      <c r="A17" s="15" t="s">
+        <v>25</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C17" s="16">
-        <f>SUM(C9:C16)</f>
-        <v>37950</v>
+        <v>2500</v>
       </c>
       <c r="D17" s="3"/>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="8"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="52"/>
+      <c r="A18" s="49" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="16">
+        <f>SUM(C14:C16)</f>
+        <v>35000</v>
+      </c>
       <c r="D18" s="3"/>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
@@ -1192,173 +1256,233 @@
     </row>
     <row r="20" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="B20" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="E20" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="F20" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="G20" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="C20" s="19" t="s">
-        <v>4</v>
-      </c>
-      <c r="D20" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
     </row>
     <row r="21" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A21" s="21" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B21" s="22"/>
       <c r="C21" s="23"/>
       <c r="D21" s="24"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
+      <c r="E21" s="24"/>
+      <c r="F21" s="24"/>
+      <c r="G21" s="24"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="25" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C22" s="26">
-        <v>102</v>
-      </c>
-      <c r="D22" s="48">
-        <f>SUM(C9:C12)*C22</f>
-        <v>45900</v>
-      </c>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
+        <v>264</v>
+      </c>
+      <c r="D22">
+        <v>152</v>
+      </c>
+      <c r="E22">
+        <v>200</v>
+      </c>
+      <c r="F22">
+        <v>240</v>
+      </c>
+      <c r="G22">
+        <f>SUM(C22:F22)</f>
+        <v>856</v>
+      </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="25" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C23" s="26">
-        <v>88</v>
-      </c>
-      <c r="D23" s="48">
-        <f>SUM(C9:C12)*C23</f>
-        <v>39600</v>
-      </c>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
+        <v>48</v>
+      </c>
+      <c r="D23">
+        <v>72</v>
+      </c>
+      <c r="E23">
+        <v>120</v>
+      </c>
+      <c r="F23">
+        <v>32</v>
+      </c>
+      <c r="G23">
+        <f t="shared" ref="G23:G26" si="0">SUM(C23:F23)</f>
+        <v>272</v>
+      </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="25" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C24" s="26">
-        <v>102</v>
-      </c>
-      <c r="D24" s="48">
-        <f>SUM(C9:C12)*C24</f>
-        <v>45900</v>
-      </c>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
+        <v>112</v>
+      </c>
+      <c r="D24">
+        <v>88</v>
+      </c>
+      <c r="E24">
+        <v>232</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="0"/>
+        <v>432</v>
+      </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="25" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C25" s="26">
-        <v>100</v>
-      </c>
-      <c r="D25" s="48">
-        <f>SUM(C9:C12)*C25</f>
-        <v>45000</v>
+        <v>336</v>
+      </c>
+      <c r="D25">
+        <v>632</v>
+      </c>
+      <c r="E25">
+        <v>265</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="0"/>
+        <v>1233</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="25" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C26" s="26">
-        <v>25</v>
-      </c>
-      <c r="D26" s="48">
-        <f>SUM(C9:C12)*C26</f>
-        <v>11250</v>
+        <v>192</v>
+      </c>
+      <c r="D26">
+        <v>184</v>
+      </c>
+      <c r="E26">
+        <v>200</v>
+      </c>
+      <c r="F26">
+        <v>120</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="0"/>
+        <v>696</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="B27" s="28"/>
-      <c r="C27" s="29"/>
-      <c r="D27" s="49">
-        <f>SUM(D23:D26)</f>
-        <v>141750</v>
+        <v>3</v>
+      </c>
+      <c r="B27" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C27" s="46">
+        <f>SUM(C22:C26)*C9</f>
+        <v>95200</v>
+      </c>
+      <c r="D27" s="46">
+        <f>SUM(D22:D26)*C10</f>
+        <v>112800</v>
+      </c>
+      <c r="E27" s="46">
+        <f>SUM(E22:E26)*C11</f>
+        <v>101700</v>
+      </c>
+      <c r="F27" s="46">
+        <f>SUM(F22:F26)*C12</f>
+        <v>58800</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="30"/>
-      <c r="B28" s="31"/>
-      <c r="C28" s="32"/>
-      <c r="D28" s="50"/>
+      <c r="A28" s="28"/>
+      <c r="B28" s="29"/>
+      <c r="C28" s="30"/>
+      <c r="D28" s="47"/>
     </row>
     <row r="29" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="33"/>
-      <c r="B33" s="34"/>
-      <c r="C33" s="35"/>
-      <c r="D33" s="36"/>
+      <c r="A33" s="31"/>
+      <c r="B33" s="32"/>
+      <c r="C33" s="33"/>
+      <c r="D33" s="34"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="37" t="s">
-        <v>13</v>
-      </c>
-      <c r="B34" s="38" t="s">
-        <v>12</v>
-      </c>
-      <c r="C34" s="39"/>
-      <c r="D34" s="49">
-        <f>D27+C13+C14+C15+C16</f>
-        <v>179250</v>
+      <c r="A34" s="35" t="s">
+        <v>10</v>
+      </c>
+      <c r="B34" s="36" t="s">
+        <v>9</v>
+      </c>
+      <c r="C34" s="37"/>
+      <c r="D34" s="46">
+        <f>SUM(C27:F27)+C18</f>
+        <v>403500</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="40"/>
+      <c r="A35" s="38"/>
       <c r="B35" s="8"/>
-      <c r="C35" s="41"/>
-      <c r="D35" s="42"/>
+      <c r="C35" s="39"/>
+      <c r="D35" s="40"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C36" s="43"/>
-      <c r="D36" s="44"/>
+      <c r="C36" s="41"/>
+      <c r="D36" s="42"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="37" t="s">
-        <v>11</v>
-      </c>
-      <c r="B40" s="38" t="s">
-        <v>12</v>
-      </c>
-      <c r="C40" s="45"/>
-      <c r="D40" s="46">
-        <v>200000</v>
+      <c r="A40" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="B40" s="36" t="s">
+        <v>9</v>
+      </c>
+      <c r="C40" s="43"/>
+      <c r="D40" s="44">
+        <v>500000</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="47"/>
-      <c r="B41" s="47"/>
+      <c r="A41" s="45"/>
+      <c r="B41" s="45"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -1372,6 +1496,5 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Se agregan fechas de revision
</commit_message>
<xml_diff>
--- a/PlanCostos_ProyectoFinal.xlsx
+++ b/PlanCostos_ProyectoFinal.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\SistemaDeRecoleccionDeBasuraInteligente\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javie\Documents\ProjectManagement\SistemaDeRecoleccionDeBasuraInteligente\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D053CAA-A0AB-4E37-85C3-7E6CD517CEAB}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8085" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21576" windowHeight="8088" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="History" sheetId="2" r:id="rId1"/>
     <sheet name="Costos" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -156,7 +157,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="6">
     <numFmt numFmtId="164" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
@@ -597,9 +598,9 @@
     </xf>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="Celda de comprobación" xfId="3" builtinId="23"/>
-    <cellStyle name="Millares" xfId="1" builtinId="3"/>
-    <cellStyle name="Moneda" xfId="2" builtinId="4"/>
+    <cellStyle name="Check Cell" xfId="3" builtinId="23"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -632,7 +633,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Imagen 2"/>
+        <xdr:cNvPr id="3" name="Imagen 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -920,22 +927,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E5" sqref="A1:E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.125" customWidth="1"/>
-    <col min="2" max="2" width="30.25" customWidth="1"/>
+    <col min="1" max="1" width="11.09765625" customWidth="1"/>
+    <col min="2" max="2" width="30.19921875" customWidth="1"/>
     <col min="3" max="3" width="34.5" customWidth="1"/>
-    <col min="4" max="4" width="41.125" customWidth="1"/>
+    <col min="4" max="4" width="41.09765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="51" t="s">
         <v>35</v>
       </c>
@@ -949,7 +956,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" s="50">
         <v>1.1000000000000001</v>
       </c>
@@ -963,7 +970,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="50">
         <v>1.2</v>
       </c>
@@ -977,7 +984,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="50">
         <v>1.3</v>
       </c>
@@ -991,7 +998,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="50"/>
       <c r="B5" s="50"/>
       <c r="C5" s="50"/>
@@ -1004,26 +1011,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A28" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.125" customWidth="1"/>
-    <col min="3" max="3" width="13.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.25" customWidth="1"/>
-    <col min="5" max="5" width="23.75" customWidth="1"/>
+    <col min="1" max="1" width="32.8984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.09765625" customWidth="1"/>
+    <col min="3" max="3" width="13.8984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.19921875" customWidth="1"/>
+    <col min="5" max="5" width="23.69921875" customWidth="1"/>
     <col min="6" max="6" width="17" customWidth="1"/>
-    <col min="7" max="7" width="18.875" customWidth="1"/>
-    <col min="11" max="11" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.8984375" customWidth="1"/>
+    <col min="11" max="11" width="11.09765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="4"/>
       <c r="B1" s="6"/>
       <c r="C1" s="53" t="s">
@@ -1033,7 +1040,7 @@
       <c r="E1" s="53"/>
       <c r="F1" s="53"/>
     </row>
-    <row r="2" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="4"/>
       <c r="B2" s="5" t="s">
         <v>19</v>
@@ -1047,7 +1054,7 @@
         <v>3108514</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="18" x14ac:dyDescent="0.35">
       <c r="A3" s="4"/>
       <c r="B3" s="5"/>
       <c r="C3" s="55" t="s">
@@ -1059,7 +1066,7 @@
         <v>3116719</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="18" x14ac:dyDescent="0.35">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="55" t="s">
@@ -1071,7 +1078,7 @@
         <v>2600752</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="18" x14ac:dyDescent="0.35">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="55" t="s">
@@ -1083,7 +1090,7 @@
         <v>33108514</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="18" x14ac:dyDescent="0.35">
       <c r="A6" s="4"/>
       <c r="B6" s="5"/>
       <c r="C6" s="53" t="s">
@@ -1093,7 +1100,7 @@
       <c r="E6" s="53"/>
       <c r="F6" s="53"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -1102,7 +1109,7 @@
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
         <v>32</v>
       </c>
@@ -1113,7 +1120,7 @@
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="12" t="s">
         <v>20</v>
       </c>
@@ -1127,7 +1134,7 @@
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="12" t="s">
         <v>21</v>
       </c>
@@ -1141,7 +1148,7 @@
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="12" t="s">
         <v>22</v>
       </c>
@@ -1155,7 +1162,7 @@
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="12" t="s">
         <v>23</v>
       </c>
@@ -1169,7 +1176,7 @@
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
         <v>33</v>
       </c>
@@ -1179,7 +1186,7 @@
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="48" t="s">
         <v>13</v>
       </c>
@@ -1193,7 +1200,7 @@
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="15" t="s">
         <v>12</v>
       </c>
@@ -1207,7 +1214,7 @@
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="15" t="s">
         <v>14</v>
       </c>
@@ -1215,13 +1222,13 @@
         <v>9</v>
       </c>
       <c r="C16" s="16">
-        <v>5000</v>
+        <v>25000</v>
       </c>
       <c r="D16" s="3"/>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="15" t="s">
         <v>25</v>
       </c>
@@ -1235,7 +1242,7 @@
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="49" t="s">
         <v>3</v>
       </c>
@@ -1244,17 +1251,17 @@
       </c>
       <c r="C18" s="16">
         <f>SUM(C14:C16)</f>
-        <v>35000</v>
+        <v>55000</v>
       </c>
       <c r="D18" s="3"/>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
     </row>
-    <row r="20" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="17" t="s">
         <v>2</v>
       </c>
@@ -1277,7 +1284,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A21" s="21" t="s">
         <v>4</v>
       </c>
@@ -1288,7 +1295,7 @@
       <c r="F21" s="24"/>
       <c r="G21" s="24"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="25" t="s">
         <v>27</v>
       </c>
@@ -1312,7 +1319,7 @@
         <v>856</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="25" t="s">
         <v>11</v>
       </c>
@@ -1336,7 +1343,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="25" t="s">
         <v>6</v>
       </c>
@@ -1360,7 +1367,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="25" t="s">
         <v>26</v>
       </c>
@@ -1384,7 +1391,7 @@
         <v>1233</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="25" t="s">
         <v>7</v>
       </c>
@@ -1408,7 +1415,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="27" t="s">
         <v>3</v>
       </c>
@@ -1432,20 +1439,20 @@
         <v>58800</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="28"/>
       <c r="B28" s="29"/>
       <c r="C28" s="30"/>
       <c r="D28" s="47"/>
     </row>
-    <row r="29" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" ht="16.2" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="31"/>
       <c r="B33" s="32"/>
       <c r="C33" s="33"/>
       <c r="D33" s="34"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="35" t="s">
         <v>10</v>
       </c>
@@ -1455,20 +1462,20 @@
       <c r="C34" s="37"/>
       <c r="D34" s="46">
         <f>SUM(C27:F27)+C18</f>
-        <v>403500</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+        <v>423500</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="38"/>
       <c r="B35" s="8"/>
       <c r="C35" s="39"/>
       <c r="D35" s="40"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C36" s="41"/>
       <c r="D36" s="42"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="35" t="s">
         <v>8</v>
       </c>
@@ -1477,10 +1484,10 @@
       </c>
       <c r="C40" s="43"/>
       <c r="D40" s="44">
-        <v>500000</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+        <v>450000</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="45"/>
       <c r="B41" s="45"/>
     </row>

</xml_diff>